<commit_message>
made date formating and date overalapping a little easier
</commit_message>
<xml_diff>
--- a/statistic_id253577_instagram_-number-of-monthly-active-users-2013-2018.xlsx
+++ b/statistic_id253577_instagram_-number-of-monthly-active-users-2013-2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivansepulveda/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivansepulveda/Documents/GitHub/FashionStockSocialMediaCorrelation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="175" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>